<commit_message>
join_elo and split_elo implemented
</commit_message>
<xml_diff>
--- a/join_thoughts.xlsx
+++ b/join_thoughts.xlsx
@@ -178,11 +178,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="213591168"/>
-        <c:axId val="213592704"/>
+        <c:axId val="142945280"/>
+        <c:axId val="160625408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="213591168"/>
+        <c:axId val="142945280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -191,7 +191,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213592704"/>
+        <c:crossAx val="160625408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -199,7 +199,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213592704"/>
+        <c:axId val="160625408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -210,14 +210,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213591168"/>
+        <c:crossAx val="142945280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -312,11 +311,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="154771456"/>
-        <c:axId val="154772992"/>
+        <c:axId val="160645504"/>
+        <c:axId val="160647040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="154771456"/>
+        <c:axId val="160645504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -325,7 +324,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154772992"/>
+        <c:crossAx val="160647040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -333,7 +332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154772992"/>
+        <c:axId val="160647040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -344,14 +343,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154771456"/>
+        <c:crossAx val="160645504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -399,7 +397,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>1138.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>755.09</c:v>
@@ -446,11 +444,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="152165760"/>
-        <c:axId val="152171648"/>
+        <c:axId val="179771264"/>
+        <c:axId val="179772800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="152165760"/>
+        <c:axId val="179771264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,7 +457,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152171648"/>
+        <c:crossAx val="179772800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -467,7 +465,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152171648"/>
+        <c:axId val="179772800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,7 +476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152165760"/>
+        <c:crossAx val="179771264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -533,7 +531,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="68"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>830</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>750</c:v>
@@ -754,7 +752,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="68"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>1200</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>760</c:v>
@@ -975,7 +973,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="68"/>
                 <c:pt idx="0">
-                  <c:v>750</c:v>
+                  <c:v>1138.21</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>755.09</c:v>
@@ -1193,11 +1191,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="157497216"/>
-        <c:axId val="157732224"/>
+        <c:axId val="179806976"/>
+        <c:axId val="179808512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="157497216"/>
+        <c:axId val="179806976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,7 +1204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157732224"/>
+        <c:crossAx val="179808512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1214,7 +1212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="157732224"/>
+        <c:axId val="179808512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="740"/>
@@ -1226,7 +1224,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="157497216"/>
+        <c:crossAx val="179806976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1354,16 +1352,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2034,7 +2032,7 @@
   <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,14 +2053,18 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>750</v>
+        <v>830</v>
       </c>
       <c r="B2">
-        <v>750</v>
+        <v>1200</v>
       </c>
       <c r="C2">
-        <f>MIN(MIN(A2:B2)+ABS(A2-B2)*0.5+(ABS(A2-B2)*$H$1)^2,MAX(B1,B2))</f>
-        <v>750</v>
+        <f>MIN(MIN(A2:B2)+ABS(A2-B2)*0.5+(ABS(A2-B2)*$H$1)^2,MAX(A2,B2))</f>
+        <v>1138.21</v>
+      </c>
+      <c r="D2">
+        <f>ABS(A2-C2)/ABS(B2-A2)</f>
+        <v>0.83300000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2073,7 +2075,7 @@
         <v>760</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C66" si="0">MIN(MIN(A3:B3)+ABS(A3-B3)*0.5+(ABS(A3-B3)*$H$1)^2,MAX(B2,B3))</f>
+        <f>MIN(MIN(A3:B3)+ABS(A3-B3)*0.5+(ABS(A3-B3)*$H$1)^2,MAX(A3,B3))</f>
         <v>755.09</v>
       </c>
       <c r="D3">
@@ -2089,7 +2091,7 @@
         <v>770</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C3:C66" si="0">MIN(MIN(A4:B4)+ABS(A4-B4)*0.5+(ABS(A4-B4)*$H$1)^2,MAX(A4,B4))</f>
         <v>760.36</v>
       </c>
       <c r="D4">
@@ -2353,11 +2355,11 @@
         <v>0.66199999999999981</v>
       </c>
       <c r="E20">
-        <f>B20-C20</f>
+        <f t="shared" ref="E20:E51" si="2">B20-C20</f>
         <v>60.840000000000032</v>
       </c>
       <c r="F20">
-        <f>A20-B20</f>
+        <f t="shared" ref="F20:F51" si="3">A20-B20</f>
         <v>-180</v>
       </c>
     </row>
@@ -2377,11 +2379,11 @@
         <v>0.67100000000000004</v>
       </c>
       <c r="E21">
-        <f>B21-C21</f>
+        <f t="shared" si="2"/>
         <v>62.509999999999991</v>
       </c>
       <c r="F21">
-        <f>A21-B21</f>
+        <f t="shared" si="3"/>
         <v>-190</v>
       </c>
     </row>
@@ -2401,11 +2403,11 @@
         <v>0.68</v>
       </c>
       <c r="E22">
-        <f>B22-C22</f>
+        <f t="shared" si="2"/>
         <v>64</v>
       </c>
       <c r="F22">
-        <f>A22-B22</f>
+        <f t="shared" si="3"/>
         <v>-200</v>
       </c>
     </row>
@@ -2425,11 +2427,11 @@
         <v>0.68900000000000028</v>
       </c>
       <c r="E23">
-        <f>B23-C23</f>
+        <f t="shared" si="2"/>
         <v>65.309999999999945</v>
       </c>
       <c r="F23">
-        <f>A23-B23</f>
+        <f t="shared" si="3"/>
         <v>-210</v>
       </c>
     </row>
@@ -2449,11 +2451,11 @@
         <v>0.69799999999999973</v>
       </c>
       <c r="E24">
-        <f>B24-C24</f>
+        <f t="shared" si="2"/>
         <v>66.440000000000055</v>
       </c>
       <c r="F24">
-        <f>A24-B24</f>
+        <f t="shared" si="3"/>
         <v>-220</v>
       </c>
     </row>
@@ -2473,11 +2475,11 @@
         <v>0.70700000000000007</v>
       </c>
       <c r="E25">
-        <f>B25-C25</f>
+        <f t="shared" si="2"/>
         <v>67.389999999999986</v>
       </c>
       <c r="F25">
-        <f>A25-B25</f>
+        <f t="shared" si="3"/>
         <v>-230</v>
       </c>
     </row>
@@ -2497,11 +2499,11 @@
         <v>0.71600000000000008</v>
       </c>
       <c r="E26">
-        <f>B26-C26</f>
+        <f t="shared" si="2"/>
         <v>68.159999999999968</v>
       </c>
       <c r="F26">
-        <f>A26-B26</f>
+        <f t="shared" si="3"/>
         <v>-240</v>
       </c>
     </row>
@@ -2521,11 +2523,11 @@
         <v>0.72499999999999998</v>
       </c>
       <c r="E27">
-        <f>B27-C27</f>
+        <f t="shared" si="2"/>
         <v>68.75</v>
       </c>
       <c r="F27">
-        <f>A27-B27</f>
+        <f t="shared" si="3"/>
         <v>-250</v>
       </c>
     </row>
@@ -2545,11 +2547,11 @@
         <v>0.7340000000000001</v>
       </c>
       <c r="E28">
-        <f>B28-C28</f>
+        <f t="shared" si="2"/>
         <v>69.159999999999968</v>
       </c>
       <c r="F28">
-        <f>A28-B28</f>
+        <f t="shared" si="3"/>
         <v>-260</v>
       </c>
     </row>
@@ -2569,11 +2571,11 @@
         <v>0.7430000000000001</v>
       </c>
       <c r="E29">
-        <f>B29-C29</f>
+        <f t="shared" si="2"/>
         <v>69.389999999999986</v>
       </c>
       <c r="F29">
-        <f>A29-B29</f>
+        <f t="shared" si="3"/>
         <v>-270</v>
       </c>
     </row>
@@ -2593,11 +2595,11 @@
         <v>0.75199999999999978</v>
       </c>
       <c r="E30">
-        <f>B30-C30</f>
+        <f t="shared" si="2"/>
         <v>69.440000000000055</v>
       </c>
       <c r="F30">
-        <f>A30-B30</f>
+        <f t="shared" si="3"/>
         <v>-280</v>
       </c>
     </row>
@@ -2617,11 +2619,11 @@
         <v>0.76099999999999979</v>
       </c>
       <c r="E31">
-        <f>B31-C31</f>
+        <f t="shared" si="2"/>
         <v>69.310000000000059</v>
       </c>
       <c r="F31">
-        <f>A31-B31</f>
+        <f t="shared" si="3"/>
         <v>-290</v>
       </c>
     </row>
@@ -2641,11 +2643,11 @@
         <v>0.77</v>
       </c>
       <c r="E32">
-        <f>B32-C32</f>
+        <f t="shared" si="2"/>
         <v>69</v>
       </c>
       <c r="F32">
-        <f>A32-B32</f>
+        <f t="shared" si="3"/>
         <v>-300</v>
       </c>
     </row>
@@ -2665,11 +2667,11 @@
         <v>0.77900000000000003</v>
       </c>
       <c r="E33">
-        <f>B33-C33</f>
+        <f t="shared" si="2"/>
         <v>68.509999999999991</v>
       </c>
       <c r="F33">
-        <f>A33-B33</f>
+        <f t="shared" si="3"/>
         <v>-310</v>
       </c>
     </row>
@@ -2689,11 +2691,11 @@
         <v>0.78799999999999992</v>
       </c>
       <c r="E34">
-        <f>B34-C34</f>
+        <f t="shared" si="2"/>
         <v>67.840000000000032</v>
       </c>
       <c r="F34">
-        <f>A34-B34</f>
+        <f t="shared" si="3"/>
         <v>-320</v>
       </c>
     </row>
@@ -2713,11 +2715,11 @@
         <v>0.79699999999999993</v>
       </c>
       <c r="E35">
-        <f>B35-C35</f>
+        <f t="shared" si="2"/>
         <v>66.990000000000009</v>
       </c>
       <c r="F35">
-        <f>A35-B35</f>
+        <f t="shared" si="3"/>
         <v>-330</v>
       </c>
     </row>
@@ -2737,11 +2739,11 @@
         <v>0.80599999999999994</v>
       </c>
       <c r="E36">
-        <f>B36-C36</f>
+        <f t="shared" si="2"/>
         <v>65.960000000000036</v>
       </c>
       <c r="F36">
-        <f>A36-B36</f>
+        <f t="shared" si="3"/>
         <v>-340</v>
       </c>
     </row>
@@ -2761,11 +2763,11 @@
         <v>0.81499999999999995</v>
       </c>
       <c r="E37">
-        <f>B37-C37</f>
+        <f t="shared" si="2"/>
         <v>64.75</v>
       </c>
       <c r="F37">
-        <f>A37-B37</f>
+        <f t="shared" si="3"/>
         <v>-350</v>
       </c>
     </row>
@@ -2785,11 +2787,11 @@
         <v>0.82399999999999962</v>
       </c>
       <c r="E38">
-        <f>B38-C38</f>
+        <f t="shared" si="2"/>
         <v>63.360000000000127</v>
       </c>
       <c r="F38">
-        <f>A38-B38</f>
+        <f t="shared" si="3"/>
         <v>-360</v>
       </c>
     </row>
@@ -2809,11 +2811,11 @@
         <v>0.83300000000000007</v>
       </c>
       <c r="E39">
-        <f>B39-C39</f>
+        <f t="shared" si="2"/>
         <v>61.789999999999964</v>
       </c>
       <c r="F39">
-        <f>A39-B39</f>
+        <f t="shared" si="3"/>
         <v>-370</v>
       </c>
     </row>
@@ -2833,11 +2835,11 @@
         <v>0.84200000000000008</v>
       </c>
       <c r="E40">
-        <f>B40-C40</f>
+        <f t="shared" si="2"/>
         <v>60.039999999999964</v>
       </c>
       <c r="F40">
-        <f>A40-B40</f>
+        <f t="shared" si="3"/>
         <v>-380</v>
       </c>
     </row>
@@ -2857,11 +2859,11 @@
         <v>0.85099999999999965</v>
       </c>
       <c r="E41">
-        <f>B41-C41</f>
+        <f t="shared" si="2"/>
         <v>58.110000000000127</v>
       </c>
       <c r="F41">
-        <f>A41-B41</f>
+        <f t="shared" si="3"/>
         <v>-390</v>
       </c>
     </row>
@@ -2881,11 +2883,11 @@
         <v>0.86</v>
       </c>
       <c r="E42">
-        <f>B42-C42</f>
+        <f t="shared" si="2"/>
         <v>56</v>
       </c>
       <c r="F42">
-        <f>A42-B42</f>
+        <f t="shared" si="3"/>
         <v>-400</v>
       </c>
     </row>
@@ -2905,11 +2907,11 @@
         <v>0.86899999999999988</v>
       </c>
       <c r="E43">
-        <f>B43-C43</f>
+        <f t="shared" si="2"/>
         <v>53.710000000000036</v>
       </c>
       <c r="F43">
-        <f>A43-B43</f>
+        <f t="shared" si="3"/>
         <v>-410</v>
       </c>
     </row>
@@ -2929,11 +2931,11 @@
         <v>0.878</v>
       </c>
       <c r="E44">
-        <f>B44-C44</f>
+        <f t="shared" si="2"/>
         <v>51.240000000000009</v>
       </c>
       <c r="F44">
-        <f>A44-B44</f>
+        <f t="shared" si="3"/>
         <v>-420</v>
       </c>
     </row>
@@ -2953,11 +2955,11 @@
         <v>0.88700000000000023</v>
       </c>
       <c r="E45">
-        <f>B45-C45</f>
+        <f t="shared" si="2"/>
         <v>48.589999999999918</v>
       </c>
       <c r="F45">
-        <f>A45-B45</f>
+        <f t="shared" si="3"/>
         <v>-430</v>
       </c>
     </row>
@@ -2977,11 +2979,11 @@
         <v>0.89600000000000002</v>
       </c>
       <c r="E46">
-        <f>B46-C46</f>
+        <f t="shared" si="2"/>
         <v>45.759999999999991</v>
       </c>
       <c r="F46">
-        <f>A46-B46</f>
+        <f t="shared" si="3"/>
         <v>-440</v>
       </c>
     </row>
@@ -3001,11 +3003,11 @@
         <v>0.90500000000000003</v>
       </c>
       <c r="E47">
-        <f>B47-C47</f>
+        <f t="shared" si="2"/>
         <v>42.75</v>
       </c>
       <c r="F47">
-        <f>A47-B47</f>
+        <f t="shared" si="3"/>
         <v>-450</v>
       </c>
     </row>
@@ -3025,11 +3027,11 @@
         <v>0.91400000000000015</v>
       </c>
       <c r="E48">
-        <f>B48-C48</f>
+        <f t="shared" si="2"/>
         <v>39.559999999999945</v>
       </c>
       <c r="F48">
-        <f>A48-B48</f>
+        <f t="shared" si="3"/>
         <v>-460</v>
       </c>
     </row>
@@ -3049,11 +3051,11 @@
         <v>0.92299999999999993</v>
       </c>
       <c r="E49">
-        <f>B49-C49</f>
+        <f t="shared" si="2"/>
         <v>36.190000000000055</v>
       </c>
       <c r="F49">
-        <f>A49-B49</f>
+        <f t="shared" si="3"/>
         <v>-470</v>
       </c>
     </row>
@@ -3073,11 +3075,11 @@
         <v>0.93199999999999983</v>
       </c>
       <c r="E50">
-        <f>B50-C50</f>
+        <f t="shared" si="2"/>
         <v>32.6400000000001</v>
       </c>
       <c r="F50">
-        <f>A50-B50</f>
+        <f t="shared" si="3"/>
         <v>-480</v>
       </c>
     </row>
@@ -3097,11 +3099,11 @@
         <v>0.94099999999999984</v>
       </c>
       <c r="E51">
-        <f>B51-C51</f>
+        <f t="shared" si="2"/>
         <v>28.910000000000082</v>
       </c>
       <c r="F51">
-        <f>A51-B51</f>
+        <f t="shared" si="3"/>
         <v>-490</v>
       </c>
     </row>
@@ -3121,11 +3123,11 @@
         <v>0.95</v>
       </c>
       <c r="E52">
-        <f>B52-C52</f>
+        <f t="shared" ref="E52:E83" si="4">B52-C52</f>
         <v>25</v>
       </c>
       <c r="F52">
-        <f>A52-B52</f>
+        <f t="shared" ref="F52:F83" si="5">A52-B52</f>
         <v>-500</v>
       </c>
     </row>
@@ -3145,11 +3147,11 @@
         <v>0.95899999999999985</v>
       </c>
       <c r="E53">
-        <f>B53-C53</f>
+        <f t="shared" si="4"/>
         <v>20.910000000000082</v>
       </c>
       <c r="F53">
-        <f>A53-B53</f>
+        <f t="shared" si="5"/>
         <v>-510</v>
       </c>
     </row>
@@ -3169,11 +3171,11 @@
         <v>0.96799999999999986</v>
       </c>
       <c r="E54">
-        <f>B54-C54</f>
+        <f t="shared" si="4"/>
         <v>16.6400000000001</v>
       </c>
       <c r="F54">
-        <f>A54-B54</f>
+        <f t="shared" si="5"/>
         <v>-520</v>
       </c>
     </row>
@@ -3193,11 +3195,11 @@
         <v>0.97699999999999987</v>
       </c>
       <c r="E55">
-        <f>B55-C55</f>
+        <f t="shared" si="4"/>
         <v>12.190000000000055</v>
       </c>
       <c r="F55">
-        <f>A55-B55</f>
+        <f t="shared" si="5"/>
         <v>-530</v>
       </c>
     </row>
@@ -3217,11 +3219,11 @@
         <v>0.9860000000000001</v>
       </c>
       <c r="E56">
-        <f>B56-C56</f>
+        <f t="shared" si="4"/>
         <v>7.5599999999999454</v>
       </c>
       <c r="F56">
-        <f>A56-B56</f>
+        <f t="shared" si="5"/>
         <v>-540</v>
       </c>
     </row>
@@ -3241,11 +3243,11 @@
         <v>0.995</v>
       </c>
       <c r="E57">
-        <f>B57-C57</f>
+        <f t="shared" si="4"/>
         <v>2.75</v>
       </c>
       <c r="F57">
-        <f>A57-B57</f>
+        <f t="shared" si="5"/>
         <v>-550</v>
       </c>
     </row>
@@ -3265,11 +3267,11 @@
         <v>1</v>
       </c>
       <c r="E58" s="2">
-        <f>B58-C58</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F58" s="2">
-        <f>A58-B58</f>
+        <f t="shared" si="5"/>
         <v>-560</v>
       </c>
     </row>
@@ -3285,11 +3287,11 @@
         <v>1320</v>
       </c>
       <c r="E59">
-        <f>B59-C59</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F59">
-        <f>A59-B59</f>
+        <f t="shared" si="5"/>
         <v>-570</v>
       </c>
     </row>
@@ -3305,11 +3307,11 @@
         <v>1330</v>
       </c>
       <c r="E60">
-        <f>B60-C60</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F60">
-        <f>A60-B60</f>
+        <f t="shared" si="5"/>
         <v>-580</v>
       </c>
     </row>
@@ -3325,11 +3327,11 @@
         <v>1340</v>
       </c>
       <c r="E61">
-        <f>B61-C61</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F61">
-        <f>A61-B61</f>
+        <f t="shared" si="5"/>
         <v>-590</v>
       </c>
     </row>
@@ -3345,11 +3347,11 @@
         <v>1350</v>
       </c>
       <c r="E62">
-        <f>B62-C62</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F62">
-        <f>A62-B62</f>
+        <f t="shared" si="5"/>
         <v>-600</v>
       </c>
     </row>
@@ -3365,11 +3367,11 @@
         <v>1360</v>
       </c>
       <c r="E63">
-        <f>B63-C63</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F63">
-        <f>A63-B63</f>
+        <f t="shared" si="5"/>
         <v>-610</v>
       </c>
     </row>
@@ -3385,11 +3387,11 @@
         <v>1370</v>
       </c>
       <c r="E64">
-        <f>B64-C64</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F64">
-        <f>A64-B64</f>
+        <f t="shared" si="5"/>
         <v>-620</v>
       </c>
     </row>
@@ -3405,11 +3407,11 @@
         <v>1380</v>
       </c>
       <c r="E65">
-        <f>B65-C65</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F65">
-        <f>A65-B65</f>
+        <f t="shared" si="5"/>
         <v>-630</v>
       </c>
     </row>
@@ -3425,11 +3427,11 @@
         <v>1390</v>
       </c>
       <c r="E66">
-        <f>B66-C66</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F66">
-        <f>A66-B66</f>
+        <f t="shared" si="5"/>
         <v>-640</v>
       </c>
     </row>
@@ -3441,15 +3443,15 @@
         <v>1400</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="2">MIN(MIN(A67:B67)+ABS(A67-B67)*0.5+(ABS(A67-B67)*$H$1)^2,MAX(B66,B67))</f>
+        <f t="shared" ref="C67:C130" si="6">MIN(MIN(A67:B67)+ABS(A67-B67)*0.5+(ABS(A67-B67)*$H$1)^2,MAX(A67,B67))</f>
         <v>1400</v>
       </c>
       <c r="E67">
-        <f>B67-C67</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F67">
-        <f>A67-B67</f>
+        <f t="shared" si="5"/>
         <v>-650</v>
       </c>
     </row>
@@ -3461,15 +3463,15 @@
         <v>1410</v>
       </c>
       <c r="C68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1410</v>
       </c>
       <c r="E68">
-        <f>B68-C68</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F68">
-        <f>A68-B68</f>
+        <f t="shared" si="5"/>
         <v>-660</v>
       </c>
     </row>
@@ -3481,15 +3483,15 @@
         <v>1420</v>
       </c>
       <c r="C69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1420</v>
       </c>
       <c r="E69">
-        <f>B69-C69</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F69">
-        <f>A69-B69</f>
+        <f t="shared" si="5"/>
         <v>-670</v>
       </c>
     </row>
@@ -3501,15 +3503,15 @@
         <v>1430</v>
       </c>
       <c r="C70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1430</v>
       </c>
       <c r="E70">
-        <f>B70-C70</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F70">
-        <f>A70-B70</f>
+        <f t="shared" si="5"/>
         <v>-680</v>
       </c>
     </row>
@@ -3521,15 +3523,15 @@
         <v>1440</v>
       </c>
       <c r="C71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1440</v>
       </c>
       <c r="E71">
-        <f>B71-C71</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F71">
-        <f>A71-B71</f>
+        <f t="shared" si="5"/>
         <v>-690</v>
       </c>
     </row>
@@ -3541,15 +3543,15 @@
         <v>1450</v>
       </c>
       <c r="C72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1450</v>
       </c>
       <c r="E72">
-        <f>B72-C72</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F72">
-        <f>A72-B72</f>
+        <f t="shared" si="5"/>
         <v>-700</v>
       </c>
     </row>
@@ -3561,15 +3563,15 @@
         <v>1460</v>
       </c>
       <c r="C73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1460</v>
       </c>
       <c r="E73">
-        <f>B73-C73</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F73">
-        <f>A73-B73</f>
+        <f t="shared" si="5"/>
         <v>-710</v>
       </c>
     </row>
@@ -3581,15 +3583,15 @@
         <v>1470</v>
       </c>
       <c r="C74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1470</v>
       </c>
       <c r="E74">
-        <f>B74-C74</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F74">
-        <f>A74-B74</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
     </row>
@@ -3601,15 +3603,15 @@
         <v>1480</v>
       </c>
       <c r="C75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1480</v>
       </c>
       <c r="E75">
-        <f>B75-C75</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F75">
-        <f>A75-B75</f>
+        <f t="shared" si="5"/>
         <v>-730</v>
       </c>
     </row>
@@ -3621,15 +3623,15 @@
         <v>1490</v>
       </c>
       <c r="C76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1490</v>
       </c>
       <c r="E76">
-        <f>B76-C76</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F76">
-        <f>A76-B76</f>
+        <f t="shared" si="5"/>
         <v>-740</v>
       </c>
     </row>
@@ -3641,15 +3643,15 @@
         <v>1500</v>
       </c>
       <c r="C77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1500</v>
       </c>
       <c r="E77">
-        <f>B77-C77</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F77">
-        <f>A77-B77</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
     </row>
@@ -3661,15 +3663,15 @@
         <v>1510</v>
       </c>
       <c r="C78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1510</v>
       </c>
       <c r="E78">
-        <f>B78-C78</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F78">
-        <f>A78-B78</f>
+        <f t="shared" si="5"/>
         <v>-760</v>
       </c>
     </row>
@@ -3681,15 +3683,15 @@
         <v>1520</v>
       </c>
       <c r="C79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1520</v>
       </c>
       <c r="E79">
-        <f>B79-C79</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F79">
-        <f>A79-B79</f>
+        <f t="shared" si="5"/>
         <v>-770</v>
       </c>
     </row>
@@ -3701,15 +3703,15 @@
         <v>1530</v>
       </c>
       <c r="C80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1530</v>
       </c>
       <c r="E80">
-        <f>B80-C80</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F80">
-        <f>A80-B80</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
     </row>
@@ -3721,15 +3723,15 @@
         <v>1540</v>
       </c>
       <c r="C81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1540</v>
       </c>
       <c r="E81">
-        <f>B81-C81</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F81">
-        <f>A81-B81</f>
+        <f t="shared" si="5"/>
         <v>-790</v>
       </c>
     </row>
@@ -3741,15 +3743,15 @@
         <v>1550</v>
       </c>
       <c r="C82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1550</v>
       </c>
       <c r="E82">
-        <f>B82-C82</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F82">
-        <f>A82-B82</f>
+        <f t="shared" si="5"/>
         <v>-800</v>
       </c>
     </row>
@@ -3761,15 +3763,15 @@
         <v>1560</v>
       </c>
       <c r="C83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1560</v>
       </c>
       <c r="E83">
-        <f>B83-C83</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F83">
-        <f>A83-B83</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
     </row>
@@ -3781,15 +3783,15 @@
         <v>1570</v>
       </c>
       <c r="C84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1570</v>
       </c>
       <c r="E84">
-        <f>B84-C84</f>
+        <f t="shared" ref="E84:E115" si="7">B84-C84</f>
         <v>0</v>
       </c>
       <c r="F84">
-        <f>A84-B84</f>
+        <f t="shared" ref="F84:F115" si="8">A84-B84</f>
         <v>-820</v>
       </c>
     </row>
@@ -3801,15 +3803,15 @@
         <v>1580</v>
       </c>
       <c r="C85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1580</v>
       </c>
       <c r="E85">
-        <f>B85-C85</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F85">
-        <f>A85-B85</f>
+        <f t="shared" si="8"/>
         <v>-830</v>
       </c>
     </row>
@@ -3821,15 +3823,15 @@
         <v>1590</v>
       </c>
       <c r="C86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1590</v>
       </c>
       <c r="E86">
-        <f>B86-C86</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F86">
-        <f>A86-B86</f>
+        <f t="shared" si="8"/>
         <v>-840</v>
       </c>
     </row>
@@ -3841,15 +3843,15 @@
         <v>1600</v>
       </c>
       <c r="C87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1600</v>
       </c>
       <c r="E87">
-        <f>B87-C87</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F87">
-        <f>A87-B87</f>
+        <f t="shared" si="8"/>
         <v>-850</v>
       </c>
     </row>
@@ -3861,15 +3863,15 @@
         <v>1610</v>
       </c>
       <c r="C88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1610</v>
       </c>
       <c r="E88">
-        <f>B88-C88</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F88">
-        <f>A88-B88</f>
+        <f t="shared" si="8"/>
         <v>-860</v>
       </c>
     </row>
@@ -3881,15 +3883,15 @@
         <v>1620</v>
       </c>
       <c r="C89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1620</v>
       </c>
       <c r="E89">
-        <f>B89-C89</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F89">
-        <f>A89-B89</f>
+        <f t="shared" si="8"/>
         <v>-870</v>
       </c>
     </row>
@@ -3901,15 +3903,15 @@
         <v>1630</v>
       </c>
       <c r="C90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1630</v>
       </c>
       <c r="E90">
-        <f>B90-C90</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F90">
-        <f>A90-B90</f>
+        <f t="shared" si="8"/>
         <v>-880</v>
       </c>
     </row>
@@ -3921,15 +3923,15 @@
         <v>1640</v>
       </c>
       <c r="C91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1640</v>
       </c>
       <c r="E91">
-        <f>B91-C91</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F91">
-        <f>A91-B91</f>
+        <f t="shared" si="8"/>
         <v>-890</v>
       </c>
     </row>
@@ -3941,15 +3943,15 @@
         <v>1650</v>
       </c>
       <c r="C92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1650</v>
       </c>
       <c r="E92">
-        <f>B92-C92</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F92">
-        <f>A92-B92</f>
+        <f t="shared" si="8"/>
         <v>-900</v>
       </c>
     </row>
@@ -3961,15 +3963,15 @@
         <v>1660</v>
       </c>
       <c r="C93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1660</v>
       </c>
       <c r="E93">
-        <f>B93-C93</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F93">
-        <f>A93-B93</f>
+        <f t="shared" si="8"/>
         <v>-910</v>
       </c>
     </row>
@@ -3981,15 +3983,15 @@
         <v>1670</v>
       </c>
       <c r="C94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1670</v>
       </c>
       <c r="E94">
-        <f>B94-C94</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F94">
-        <f>A94-B94</f>
+        <f t="shared" si="8"/>
         <v>-920</v>
       </c>
     </row>
@@ -4001,15 +4003,15 @@
         <v>1680</v>
       </c>
       <c r="C95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1680</v>
       </c>
       <c r="E95">
-        <f>B95-C95</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F95">
-        <f>A95-B95</f>
+        <f t="shared" si="8"/>
         <v>-930</v>
       </c>
     </row>
@@ -4021,15 +4023,15 @@
         <v>1690</v>
       </c>
       <c r="C96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1690</v>
       </c>
       <c r="E96">
-        <f>B96-C96</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F96">
-        <f>A96-B96</f>
+        <f t="shared" si="8"/>
         <v>-940</v>
       </c>
     </row>
@@ -4041,15 +4043,15 @@
         <v>1700</v>
       </c>
       <c r="C97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1700</v>
       </c>
       <c r="E97">
-        <f>B97-C97</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F97">
-        <f>A97-B97</f>
+        <f t="shared" si="8"/>
         <v>-950</v>
       </c>
     </row>
@@ -4061,15 +4063,15 @@
         <v>1710</v>
       </c>
       <c r="C98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1710</v>
       </c>
       <c r="E98">
-        <f>B98-C98</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F98">
-        <f>A98-B98</f>
+        <f t="shared" si="8"/>
         <v>-960</v>
       </c>
     </row>
@@ -4081,15 +4083,15 @@
         <v>1720</v>
       </c>
       <c r="C99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1720</v>
       </c>
       <c r="E99">
-        <f>B99-C99</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F99">
-        <f>A99-B99</f>
+        <f t="shared" si="8"/>
         <v>-970</v>
       </c>
     </row>
@@ -4101,15 +4103,15 @@
         <v>1730</v>
       </c>
       <c r="C100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1730</v>
       </c>
       <c r="E100">
-        <f>B100-C100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F100">
-        <f>A100-B100</f>
+        <f t="shared" si="8"/>
         <v>-980</v>
       </c>
     </row>
@@ -4121,15 +4123,15 @@
         <v>1740</v>
       </c>
       <c r="C101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1740</v>
       </c>
       <c r="E101">
-        <f>B101-C101</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F101">
-        <f>A101-B101</f>
+        <f t="shared" si="8"/>
         <v>-990</v>
       </c>
     </row>
@@ -4141,15 +4143,15 @@
         <v>1750</v>
       </c>
       <c r="C102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1750</v>
       </c>
       <c r="E102">
-        <f>B102-C102</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F102">
-        <f>A102-B102</f>
+        <f t="shared" si="8"/>
         <v>-1000</v>
       </c>
     </row>
@@ -4161,15 +4163,15 @@
         <v>1760</v>
       </c>
       <c r="C103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1760</v>
       </c>
       <c r="E103">
-        <f>B103-C103</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F103">
-        <f>A103-B103</f>
+        <f t="shared" si="8"/>
         <v>-1010</v>
       </c>
     </row>
@@ -4181,15 +4183,15 @@
         <v>1770</v>
       </c>
       <c r="C104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1770</v>
       </c>
       <c r="E104">
-        <f>B104-C104</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F104">
-        <f>A104-B104</f>
+        <f t="shared" si="8"/>
         <v>-1020</v>
       </c>
     </row>
@@ -4201,15 +4203,15 @@
         <v>1780</v>
       </c>
       <c r="C105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1780</v>
       </c>
       <c r="E105">
-        <f>B105-C105</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F105">
-        <f>A105-B105</f>
+        <f t="shared" si="8"/>
         <v>-1030</v>
       </c>
     </row>
@@ -4221,15 +4223,15 @@
         <v>1790</v>
       </c>
       <c r="C106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1790</v>
       </c>
       <c r="E106">
-        <f>B106-C106</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F106">
-        <f>A106-B106</f>
+        <f t="shared" si="8"/>
         <v>-1040</v>
       </c>
     </row>
@@ -4241,15 +4243,15 @@
         <v>1800</v>
       </c>
       <c r="C107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1800</v>
       </c>
       <c r="E107">
-        <f>B107-C107</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F107">
-        <f>A107-B107</f>
+        <f t="shared" si="8"/>
         <v>-1050</v>
       </c>
     </row>
@@ -4261,15 +4263,15 @@
         <v>1810</v>
       </c>
       <c r="C108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1810</v>
       </c>
       <c r="E108">
-        <f>B108-C108</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F108">
-        <f>A108-B108</f>
+        <f t="shared" si="8"/>
         <v>-1060</v>
       </c>
     </row>
@@ -4281,15 +4283,15 @@
         <v>1820</v>
       </c>
       <c r="C109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1820</v>
       </c>
       <c r="E109">
-        <f>B109-C109</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F109">
-        <f>A109-B109</f>
+        <f t="shared" si="8"/>
         <v>-1070</v>
       </c>
     </row>
@@ -4301,15 +4303,15 @@
         <v>1830</v>
       </c>
       <c r="C110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1830</v>
       </c>
       <c r="E110">
-        <f>B110-C110</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F110">
-        <f>A110-B110</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
     </row>
@@ -4321,15 +4323,15 @@
         <v>1840</v>
       </c>
       <c r="C111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1840</v>
       </c>
       <c r="E111">
-        <f>B111-C111</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F111">
-        <f>A111-B111</f>
+        <f t="shared" si="8"/>
         <v>-1090</v>
       </c>
     </row>
@@ -4341,15 +4343,15 @@
         <v>1850</v>
       </c>
       <c r="C112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1850</v>
       </c>
       <c r="E112">
-        <f>B112-C112</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F112">
-        <f>A112-B112</f>
+        <f t="shared" si="8"/>
         <v>-1100</v>
       </c>
     </row>
@@ -4361,15 +4363,15 @@
         <v>1860</v>
       </c>
       <c r="C113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1860</v>
       </c>
       <c r="E113">
-        <f>B113-C113</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F113">
-        <f>A113-B113</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
     </row>
@@ -4381,15 +4383,15 @@
         <v>1870</v>
       </c>
       <c r="C114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1870</v>
       </c>
       <c r="E114">
-        <f>B114-C114</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F114">
-        <f>A114-B114</f>
+        <f t="shared" si="8"/>
         <v>-1120</v>
       </c>
     </row>
@@ -4401,15 +4403,15 @@
         <v>1880</v>
       </c>
       <c r="C115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1880</v>
       </c>
       <c r="E115">
-        <f>B115-C115</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="F115">
-        <f>A115-B115</f>
+        <f t="shared" si="8"/>
         <v>-1130</v>
       </c>
     </row>
@@ -4421,15 +4423,15 @@
         <v>1890</v>
       </c>
       <c r="C116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1890</v>
       </c>
       <c r="E116">
-        <f>B116-C116</f>
+        <f t="shared" ref="E116:E147" si="9">B116-C116</f>
         <v>0</v>
       </c>
       <c r="F116">
-        <f>A116-B116</f>
+        <f t="shared" ref="F116:F147" si="10">A116-B116</f>
         <v>-1140</v>
       </c>
     </row>
@@ -4441,15 +4443,15 @@
         <v>1900</v>
       </c>
       <c r="C117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1900</v>
       </c>
       <c r="E117">
-        <f>B117-C117</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F117">
-        <f>A117-B117</f>
+        <f t="shared" si="10"/>
         <v>-1150</v>
       </c>
     </row>
@@ -4461,15 +4463,15 @@
         <v>1910</v>
       </c>
       <c r="C118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1910</v>
       </c>
       <c r="E118">
-        <f>B118-C118</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F118">
-        <f>A118-B118</f>
+        <f t="shared" si="10"/>
         <v>-1160</v>
       </c>
     </row>
@@ -4481,15 +4483,15 @@
         <v>1920</v>
       </c>
       <c r="C119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1920</v>
       </c>
       <c r="E119">
-        <f>B119-C119</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F119">
-        <f>A119-B119</f>
+        <f t="shared" si="10"/>
         <v>-1170</v>
       </c>
     </row>
@@ -4501,15 +4503,15 @@
         <v>1930</v>
       </c>
       <c r="C120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1930</v>
       </c>
       <c r="E120">
-        <f>B120-C120</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F120">
-        <f>A120-B120</f>
+        <f t="shared" si="10"/>
         <v>-1180</v>
       </c>
     </row>
@@ -4521,15 +4523,15 @@
         <v>1940</v>
       </c>
       <c r="C121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1940</v>
       </c>
       <c r="E121">
-        <f>B121-C121</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F121">
-        <f>A121-B121</f>
+        <f t="shared" si="10"/>
         <v>-1190</v>
       </c>
     </row>
@@ -4541,15 +4543,15 @@
         <v>1950</v>
       </c>
       <c r="C122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1950</v>
       </c>
       <c r="E122">
-        <f>B122-C122</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F122">
-        <f>A122-B122</f>
+        <f t="shared" si="10"/>
         <v>-1200</v>
       </c>
     </row>
@@ -4561,15 +4563,15 @@
         <v>1960</v>
       </c>
       <c r="C123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1960</v>
       </c>
       <c r="E123">
-        <f>B123-C123</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F123">
-        <f>A123-B123</f>
+        <f t="shared" si="10"/>
         <v>-1210</v>
       </c>
     </row>
@@ -4581,15 +4583,15 @@
         <v>1970</v>
       </c>
       <c r="C124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1970</v>
       </c>
       <c r="E124">
-        <f>B124-C124</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F124">
-        <f>A124-B124</f>
+        <f t="shared" si="10"/>
         <v>-1220</v>
       </c>
     </row>
@@ -4601,15 +4603,15 @@
         <v>1980</v>
       </c>
       <c r="C125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1980</v>
       </c>
       <c r="E125">
-        <f>B125-C125</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F125">
-        <f>A125-B125</f>
+        <f t="shared" si="10"/>
         <v>-1230</v>
       </c>
     </row>
@@ -4621,15 +4623,15 @@
         <v>1990</v>
       </c>
       <c r="C126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1990</v>
       </c>
       <c r="E126">
-        <f>B126-C126</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F126">
-        <f>A126-B126</f>
+        <f t="shared" si="10"/>
         <v>-1240</v>
       </c>
     </row>
@@ -4641,15 +4643,15 @@
         <v>2000</v>
       </c>
       <c r="C127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2000</v>
       </c>
       <c r="E127">
-        <f>B127-C127</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F127">
-        <f>A127-B127</f>
+        <f t="shared" si="10"/>
         <v>-1250</v>
       </c>
     </row>
@@ -4661,15 +4663,15 @@
         <v>2010</v>
       </c>
       <c r="C128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2010</v>
       </c>
       <c r="E128">
-        <f>B128-C128</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F128">
-        <f>A128-B128</f>
+        <f t="shared" si="10"/>
         <v>-1260</v>
       </c>
     </row>
@@ -4681,15 +4683,15 @@
         <v>2020</v>
       </c>
       <c r="C129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2020</v>
       </c>
       <c r="E129">
-        <f>B129-C129</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F129">
-        <f>A129-B129</f>
+        <f t="shared" si="10"/>
         <v>-1270</v>
       </c>
     </row>
@@ -4701,15 +4703,15 @@
         <v>2030</v>
       </c>
       <c r="C130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>2030</v>
       </c>
       <c r="E130">
-        <f>B130-C130</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F130">
-        <f>A130-B130</f>
+        <f t="shared" si="10"/>
         <v>-1280</v>
       </c>
     </row>
@@ -4721,15 +4723,15 @@
         <v>2040</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C163" si="3">MIN(MIN(A131:B131)+ABS(A131-B131)*0.5+(ABS(A131-B131)*$H$1)^2,MAX(B130,B131))</f>
+        <f t="shared" ref="C131:C163" si="11">MIN(MIN(A131:B131)+ABS(A131-B131)*0.5+(ABS(A131-B131)*$H$1)^2,MAX(A131,B131))</f>
         <v>2040</v>
       </c>
       <c r="E131">
-        <f>B131-C131</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F131">
-        <f>A131-B131</f>
+        <f t="shared" si="10"/>
         <v>-1290</v>
       </c>
     </row>
@@ -4741,15 +4743,15 @@
         <v>2050</v>
       </c>
       <c r="C132">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2050</v>
       </c>
       <c r="E132">
-        <f>B132-C132</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F132">
-        <f>A132-B132</f>
+        <f t="shared" si="10"/>
         <v>-1300</v>
       </c>
     </row>
@@ -4761,15 +4763,15 @@
         <v>2060</v>
       </c>
       <c r="C133">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2060</v>
       </c>
       <c r="E133">
-        <f>B133-C133</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F133">
-        <f>A133-B133</f>
+        <f t="shared" si="10"/>
         <v>-1310</v>
       </c>
     </row>
@@ -4781,15 +4783,15 @@
         <v>2070</v>
       </c>
       <c r="C134">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2070</v>
       </c>
       <c r="E134">
-        <f>B134-C134</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F134">
-        <f>A134-B134</f>
+        <f t="shared" si="10"/>
         <v>-1320</v>
       </c>
     </row>
@@ -4801,15 +4803,15 @@
         <v>2080</v>
       </c>
       <c r="C135">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2080</v>
       </c>
       <c r="E135">
-        <f>B135-C135</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F135">
-        <f>A135-B135</f>
+        <f t="shared" si="10"/>
         <v>-1330</v>
       </c>
     </row>
@@ -4821,15 +4823,15 @@
         <v>2090</v>
       </c>
       <c r="C136">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2090</v>
       </c>
       <c r="E136">
-        <f>B136-C136</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F136">
-        <f>A136-B136</f>
+        <f t="shared" si="10"/>
         <v>-1340</v>
       </c>
     </row>
@@ -4841,15 +4843,15 @@
         <v>2100</v>
       </c>
       <c r="C137">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2100</v>
       </c>
       <c r="E137">
-        <f>B137-C137</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F137">
-        <f>A137-B137</f>
+        <f t="shared" si="10"/>
         <v>-1350</v>
       </c>
     </row>
@@ -4861,15 +4863,15 @@
         <v>2110</v>
       </c>
       <c r="C138">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2110</v>
       </c>
       <c r="E138">
-        <f>B138-C138</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F138">
-        <f>A138-B138</f>
+        <f t="shared" si="10"/>
         <v>-1360</v>
       </c>
     </row>
@@ -4881,15 +4883,15 @@
         <v>2120</v>
       </c>
       <c r="C139">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2120</v>
       </c>
       <c r="E139">
-        <f>B139-C139</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F139">
-        <f>A139-B139</f>
+        <f t="shared" si="10"/>
         <v>-1370</v>
       </c>
     </row>
@@ -4901,15 +4903,15 @@
         <v>2130</v>
       </c>
       <c r="C140">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2130</v>
       </c>
       <c r="E140">
-        <f>B140-C140</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F140">
-        <f>A140-B140</f>
+        <f t="shared" si="10"/>
         <v>-1380</v>
       </c>
     </row>
@@ -4921,15 +4923,15 @@
         <v>2140</v>
       </c>
       <c r="C141">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2140</v>
       </c>
       <c r="E141">
-        <f>B141-C141</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F141">
-        <f>A141-B141</f>
+        <f t="shared" si="10"/>
         <v>-1390</v>
       </c>
     </row>
@@ -4941,15 +4943,15 @@
         <v>2150</v>
       </c>
       <c r="C142">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2150</v>
       </c>
       <c r="E142">
-        <f>B142-C142</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F142">
-        <f>A142-B142</f>
+        <f t="shared" si="10"/>
         <v>-1400</v>
       </c>
     </row>
@@ -4961,15 +4963,15 @@
         <v>2160</v>
       </c>
       <c r="C143">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2160</v>
       </c>
       <c r="E143">
-        <f>B143-C143</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F143">
-        <f>A143-B143</f>
+        <f t="shared" si="10"/>
         <v>-1410</v>
       </c>
     </row>
@@ -4981,15 +4983,15 @@
         <v>2170</v>
       </c>
       <c r="C144">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2170</v>
       </c>
       <c r="E144">
-        <f>B144-C144</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F144">
-        <f>A144-B144</f>
+        <f t="shared" si="10"/>
         <v>-1420</v>
       </c>
     </row>
@@ -5001,15 +5003,15 @@
         <v>2180</v>
       </c>
       <c r="C145">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2180</v>
       </c>
       <c r="E145">
-        <f>B145-C145</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F145">
-        <f>A145-B145</f>
+        <f t="shared" si="10"/>
         <v>-1430</v>
       </c>
     </row>
@@ -5021,15 +5023,15 @@
         <v>2190</v>
       </c>
       <c r="C146">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2190</v>
       </c>
       <c r="E146">
-        <f>B146-C146</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F146">
-        <f>A146-B146</f>
+        <f t="shared" si="10"/>
         <v>-1440</v>
       </c>
     </row>
@@ -5041,15 +5043,15 @@
         <v>2200</v>
       </c>
       <c r="C147">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2200</v>
       </c>
       <c r="E147">
-        <f>B147-C147</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="F147">
-        <f>A147-B147</f>
+        <f t="shared" si="10"/>
         <v>-1450</v>
       </c>
     </row>
@@ -5061,15 +5063,15 @@
         <v>2210</v>
       </c>
       <c r="C148">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2210</v>
       </c>
       <c r="E148">
-        <f>B148-C148</f>
+        <f t="shared" ref="E148:E163" si="12">B148-C148</f>
         <v>0</v>
       </c>
       <c r="F148">
-        <f>A148-B148</f>
+        <f t="shared" ref="F148:F163" si="13">A148-B148</f>
         <v>-1460</v>
       </c>
     </row>
@@ -5081,15 +5083,15 @@
         <v>2220</v>
       </c>
       <c r="C149">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2220</v>
       </c>
       <c r="E149">
-        <f>B149-C149</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F149">
-        <f>A149-B149</f>
+        <f t="shared" si="13"/>
         <v>-1470</v>
       </c>
     </row>
@@ -5101,15 +5103,15 @@
         <v>2230</v>
       </c>
       <c r="C150">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2230</v>
       </c>
       <c r="E150">
-        <f>B150-C150</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F150">
-        <f>A150-B150</f>
+        <f t="shared" si="13"/>
         <v>-1480</v>
       </c>
     </row>
@@ -5121,15 +5123,15 @@
         <v>2240</v>
       </c>
       <c r="C151">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2240</v>
       </c>
       <c r="E151">
-        <f>B151-C151</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F151">
-        <f>A151-B151</f>
+        <f t="shared" si="13"/>
         <v>-1490</v>
       </c>
     </row>
@@ -5141,15 +5143,15 @@
         <v>2250</v>
       </c>
       <c r="C152">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2250</v>
       </c>
       <c r="E152">
-        <f>B152-C152</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F152">
-        <f>A152-B152</f>
+        <f t="shared" si="13"/>
         <v>-1500</v>
       </c>
     </row>
@@ -5161,15 +5163,15 @@
         <v>2260</v>
       </c>
       <c r="C153">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2260</v>
       </c>
       <c r="E153">
-        <f>B153-C153</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F153">
-        <f>A153-B153</f>
+        <f t="shared" si="13"/>
         <v>-1510</v>
       </c>
     </row>
@@ -5181,15 +5183,15 @@
         <v>2270</v>
       </c>
       <c r="C154">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2270</v>
       </c>
       <c r="E154">
-        <f>B154-C154</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F154">
-        <f>A154-B154</f>
+        <f t="shared" si="13"/>
         <v>-1520</v>
       </c>
     </row>
@@ -5201,15 +5203,15 @@
         <v>2280</v>
       </c>
       <c r="C155">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2280</v>
       </c>
       <c r="E155">
-        <f>B155-C155</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F155">
-        <f>A155-B155</f>
+        <f t="shared" si="13"/>
         <v>-1530</v>
       </c>
     </row>
@@ -5221,15 +5223,15 @@
         <v>2290</v>
       </c>
       <c r="C156">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2290</v>
       </c>
       <c r="E156">
-        <f>B156-C156</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F156">
-        <f>A156-B156</f>
+        <f t="shared" si="13"/>
         <v>-1540</v>
       </c>
     </row>
@@ -5241,15 +5243,15 @@
         <v>2300</v>
       </c>
       <c r="C157">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2300</v>
       </c>
       <c r="E157">
-        <f>B157-C157</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F157">
-        <f>A157-B157</f>
+        <f t="shared" si="13"/>
         <v>-1550</v>
       </c>
     </row>
@@ -5261,15 +5263,15 @@
         <v>2310</v>
       </c>
       <c r="C158">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2310</v>
       </c>
       <c r="E158">
-        <f>B158-C158</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F158">
-        <f>A158-B158</f>
+        <f t="shared" si="13"/>
         <v>-1560</v>
       </c>
     </row>
@@ -5281,15 +5283,15 @@
         <v>2320</v>
       </c>
       <c r="C159">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2320</v>
       </c>
       <c r="E159">
-        <f>B159-C159</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F159">
-        <f>A159-B159</f>
+        <f t="shared" si="13"/>
         <v>-1570</v>
       </c>
     </row>
@@ -5301,15 +5303,15 @@
         <v>2330</v>
       </c>
       <c r="C160">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2330</v>
       </c>
       <c r="E160">
-        <f>B160-C160</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F160">
-        <f>A160-B160</f>
+        <f t="shared" si="13"/>
         <v>-1580</v>
       </c>
     </row>
@@ -5321,15 +5323,15 @@
         <v>2340</v>
       </c>
       <c r="C161">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2340</v>
       </c>
       <c r="E161">
-        <f>B161-C161</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F161">
-        <f>A161-B161</f>
+        <f t="shared" si="13"/>
         <v>-1590</v>
       </c>
     </row>
@@ -5341,15 +5343,15 @@
         <v>2350</v>
       </c>
       <c r="C162">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2350</v>
       </c>
       <c r="E162">
-        <f>B162-C162</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F162">
-        <f>A162-B162</f>
+        <f t="shared" si="13"/>
         <v>-1600</v>
       </c>
     </row>
@@ -5361,15 +5363,15 @@
         <v>2360</v>
       </c>
       <c r="C163">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>2360</v>
       </c>
       <c r="E163">
-        <f>B163-C163</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="F163">
-        <f>A163-B163</f>
+        <f t="shared" si="13"/>
         <v>-1610</v>
       </c>
     </row>

</xml_diff>